<commit_message>
adding some new LDCs + renaming old ones + updating watum19
</commit_message>
<xml_diff>
--- a/watum_development_mode.xlsx
+++ b/watum_development_mode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -1658,15 +1658,6 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="39" borderId="12" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1680,6 +1671,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1818,45 +1818,6 @@
           <color rgb="FFB2B2B2"/>
         </right>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="7"/>
-        <name val="Cutive Mono"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Cutive Mono"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2204,6 +2165,45 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cutive Mono"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="7"/>
+        <name val="Cutive Mono"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4334,48 +4334,48 @@
     <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="19" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="3"/>
-    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="18"/>
+    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="18" dataCellStyle="Note">
+    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="16" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="17" dataCellStyle="Note">
+    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="15" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Tp]]-AN2)*3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Time Cell" dataDxfId="16" dataCellStyle="Note">
+    <tableColumn id="27" name="Time Cell" dataDxfId="14" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="End Spatial Cell" dataDxfId="15" dataCellStyle="Note">
+    <tableColumn id="37" name="End Spatial Cell" dataDxfId="13" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="14" dataCellStyle="Note">
+    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="12" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Delta T" dataDxfId="13" dataCellStyle="Note">
+    <tableColumn id="28" name="Delta T" dataDxfId="11" dataCellStyle="Note">
       <calculatedColumnFormula>Delta_T__seconds</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="Error Ti" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="29" name="Error Ti" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="Error Tp" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="30" name="Error Tp" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="Error Tt" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="31" name="Error Tt" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="Column1" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="32" name="Column1" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="Vi" dataDxfId="8" dataCellStyle="Note">
+    <tableColumn id="33" name="Vi" dataDxfId="6" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="delta Tp" dataDxfId="7" dataCellStyle="Note">
+    <tableColumn id="34" name="delta Tp" dataDxfId="5" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="Column2" dataDxfId="6" dataCellStyle="Note"/>
-    <tableColumn id="36" name="Column3" dataDxfId="5" dataCellStyle="Note">
+    <tableColumn id="35" name="Column2" dataDxfId="4" dataCellStyle="Note"/>
+    <tableColumn id="36" name="Column3" dataDxfId="3" dataCellStyle="Note">
       <calculatedColumnFormula>'Reach Propertise'!$F2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="40" name="Column4" dataDxfId="2" dataCellStyle="Note"/>
@@ -4683,7 +4683,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7083,9 +7083,9 @@
   </sheetPr>
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO15" sqref="AO15"/>
+      <selection pane="bottomLeft" activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7199,7 +7199,7 @@
       <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="98" t="s">
+      <c r="X1" s="95" t="s">
         <v>116</v>
       </c>
       <c r="Y1" s="17" t="s">
@@ -7250,10 +7250,10 @@
       <c r="AN1" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="AO1" s="101" t="s">
+      <c r="AO1" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="AP1" s="101" t="s">
+      <c r="AP1" s="98" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7326,7 +7326,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>1.21</v>
       </c>
-      <c r="X2" s="99">
+      <c r="X2" s="96">
         <v>1.0510314000000001</v>
       </c>
       <c r="Y2" s="76" t="str">
@@ -7391,11 +7391,11 @@
       <c r="AN2" s="75">
         <v>0</v>
       </c>
-      <c r="AO2" s="102">
+      <c r="AO2" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>1</v>
       </c>
-      <c r="AP2" s="102">
+      <c r="AP2" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7470,7 +7470,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>2.1749999999999998</v>
       </c>
-      <c r="X3" s="99">
+      <c r="X3" s="96">
         <v>0.22527449999999999</v>
       </c>
       <c r="Y3" s="76" t="str">
@@ -7535,11 +7535,11 @@
       <c r="AN3" s="75">
         <v>1</v>
       </c>
-      <c r="AO3" s="102">
+      <c r="AO3" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>2</v>
       </c>
-      <c r="AP3" s="102">
+      <c r="AP3" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7614,7 +7614,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>3.875</v>
       </c>
-      <c r="X4" s="100">
+      <c r="X4" s="97">
         <v>0.11053590000000001</v>
       </c>
       <c r="Y4" s="76" t="str">
@@ -7675,11 +7675,11 @@
         <v>1.1333</v>
       </c>
       <c r="AN4" s="75"/>
-      <c r="AO4" s="102">
+      <c r="AO4" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>3</v>
       </c>
-      <c r="AP4" s="102">
+      <c r="AP4" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7754,7 +7754,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>6.2750000000000004</v>
       </c>
-      <c r="X5" s="100">
+      <c r="X5" s="97">
         <v>5.8002699999999997E-2</v>
       </c>
       <c r="Y5" s="76" t="str">
@@ -7815,11 +7815,11 @@
         <v>2.4666999999999999</v>
       </c>
       <c r="AN5" s="75"/>
-      <c r="AO5" s="102">
+      <c r="AO5" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>6</v>
       </c>
-      <c r="AP5" s="102">
+      <c r="AP5" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7894,7 +7894,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>8.7750000000000004</v>
       </c>
-      <c r="X6" s="100">
+      <c r="X6" s="97">
         <v>3.4605400000000001E-2</v>
       </c>
       <c r="Y6" s="76" t="str">
@@ -7955,11 +7955,11 @@
         <v>3.7332999999999998</v>
       </c>
       <c r="AN6" s="75"/>
-      <c r="AO6" s="102">
+      <c r="AO6" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>8</v>
       </c>
-      <c r="AP6" s="102">
+      <c r="AP6" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8034,7 +8034,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>11.275</v>
       </c>
-      <c r="X7" s="100">
+      <c r="X7" s="97">
         <v>2.1080000000000002E-2</v>
       </c>
       <c r="Y7" s="76" t="str">
@@ -8095,11 +8095,11 @@
         <v>5.0332999999999997</v>
       </c>
       <c r="AN7" s="75"/>
-      <c r="AO7" s="102">
+      <c r="AO7" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>11</v>
       </c>
-      <c r="AP7" s="102">
+      <c r="AP7" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8174,7 +8174,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>14.775</v>
       </c>
-      <c r="X8" s="100">
+      <c r="X8" s="97">
         <v>2.0655E-2</v>
       </c>
       <c r="Y8" s="76" t="str">
@@ -8235,11 +8235,11 @@
         <v>6.5369000000000002</v>
       </c>
       <c r="AN8" s="75"/>
-      <c r="AO8" s="102">
+      <c r="AO8" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>14</v>
       </c>
-      <c r="AP8" s="102">
+      <c r="AP8" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8441,8 +8441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9752,15 +9752,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="44"/>
-      <c r="G28" s="95" t="s">
+      <c r="G28" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="97"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="102"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="45" t="s">

</xml_diff>

<commit_message>
all brand new longitudinal dispersion coefficients
</commit_message>
<xml_diff>
--- a/watum_development_mode.xlsx
+++ b/watum_development_mode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -4682,7 +4682,7 @@
   </sheetPr>
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -8441,8 +8441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Watum model just got updated
</commit_message>
<xml_diff>
--- a/watum_development_mode.xlsx
+++ b/watum_development_mode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
   <si>
     <t>Project Name</t>
   </si>
@@ -456,6 +456,18 @@
   </si>
   <si>
     <t>Li et al. (1998) [1]</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>Working?</t>
+  </si>
+  <si>
+    <t>Nay :X</t>
+  </si>
+  <si>
+    <t>Yay :D</t>
   </si>
 </sst>
 </file>
@@ -723,12 +735,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cutive Mono"/>
@@ -754,9 +760,16 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1403,7 +1416,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1591,45 +1604,45 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="38" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1640,38 +1653,43 @@
     <xf numFmtId="164" fontId="20" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="43" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="43" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="39" borderId="12" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="39" borderId="7" xfId="37" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="43" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1681,9 +1699,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1732,7 +1747,73 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4303,93 +4384,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AP8" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Note" dataCellStyle="Note">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AP8" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47" headerRowCellStyle="Note" dataCellStyle="Note">
   <autoFilter ref="A1:AP8"/>
   <tableColumns count="42">
-    <tableColumn id="1" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="40"/>
-    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="39" dataCellStyle="Note"/>
-    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="38"/>
-    <tableColumn id="5" name="Ti" dataDxfId="37" dataCellStyle="Note"/>
-    <tableColumn id="6" name="Tp" dataDxfId="36"/>
-    <tableColumn id="7" name="Tt" dataDxfId="35" dataCellStyle="Note"/>
-    <tableColumn id="8" name="Q average" dataDxfId="34" dataCellStyle="Note"/>
-    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="33" dataCellStyle="Note"/>
-    <tableColumn id="10" name="longitudinal slope" dataDxfId="32"/>
-    <tableColumn id="11" name="depth [meters]" dataDxfId="31"/>
-    <tableColumn id="12" name="width [meters]" dataDxfId="30"/>
-    <tableColumn id="13" name="Cup" dataDxfId="29"/>
-    <tableColumn id="14" name="Inj Mass" dataDxfId="28" dataCellStyle="Note"/>
-    <tableColumn id="15" name="R ratio" dataDxfId="27" dataCellStyle="Note"/>
-    <tableColumn id="16" name="Ref" dataDxfId="26" dataCellStyle="Note"/>
-    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="25">
+    <tableColumn id="1" name="Name" dataDxfId="46"/>
+    <tableColumn id="2" name="Start point distance [meters]" dataDxfId="45"/>
+    <tableColumn id="3" name="End Point distance  [meters]" dataDxfId="44" dataCellStyle="Note"/>
+    <tableColumn id="4" name="Q [m3/sec]" dataDxfId="43"/>
+    <tableColumn id="5" name="Ti" dataDxfId="42" dataCellStyle="Note"/>
+    <tableColumn id="6" name="Tp" dataDxfId="41"/>
+    <tableColumn id="7" name="Tt" dataDxfId="40" dataCellStyle="Note"/>
+    <tableColumn id="8" name="Q average" dataDxfId="39" dataCellStyle="Note"/>
+    <tableColumn id="9" name="Drainage Area [km2]" dataDxfId="38" dataCellStyle="Note"/>
+    <tableColumn id="10" name="longitudinal slope" dataDxfId="37"/>
+    <tableColumn id="11" name="depth [meters]" dataDxfId="36"/>
+    <tableColumn id="12" name="width [meters]" dataDxfId="35"/>
+    <tableColumn id="13" name="Cup" dataDxfId="34"/>
+    <tableColumn id="14" name="Inj Mass" dataDxfId="33" dataCellStyle="Note"/>
+    <tableColumn id="15" name="R ratio" dataDxfId="32" dataCellStyle="Note"/>
+    <tableColumn id="16" name="Ref" dataDxfId="31" dataCellStyle="Note"/>
+    <tableColumn id="17" name="Calculated Velocity [meters/sec]" dataDxfId="30">
       <calculatedColumnFormula>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="calculated time [hours]" dataDxfId="24" dataCellStyle="Note">
+    <tableColumn id="18" name="calculated time [hours]" dataDxfId="29" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="23" dataCellStyle="Note">
+    <tableColumn id="19" name="Observed Velocity [meters / seconds]" dataDxfId="28" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="ɳ" dataDxfId="22"/>
-    <tableColumn id="21" name="river side slope" dataDxfId="21"/>
-    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="20"/>
-    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="19" dataCellStyle="Note">
+    <tableColumn id="20" name="ɳ" dataDxfId="27"/>
+    <tableColumn id="21" name="river side slope" dataDxfId="26"/>
+    <tableColumn id="22" name="Initial Concentration [mgr/Lit]" dataDxfId="25"/>
+    <tableColumn id="23" name="End Point of Reach [km]" dataDxfId="24" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="18"/>
-    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="24" name="Only Observed Concentration (if you had losses and want to use formula look @ AP column) PPM" dataDxfId="23"/>
+    <tableColumn id="25" name="Error in Calc time Vs Obs Time" dataDxfId="22" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="16" dataCellStyle="Note">
+    <tableColumn id="26" name="Reach Length [meters]" dataDxfId="21" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="15" dataCellStyle="Note">
+    <tableColumn id="39" name="Reach Time (seconds)" dataDxfId="20" dataCellStyle="Note">
       <calculatedColumnFormula>(Table1[[#This Row],[Tp]]-AN2)*3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Time Cell" dataDxfId="14" dataCellStyle="Note">
+    <tableColumn id="27" name="Time Cell" dataDxfId="19" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="End Spatial Cell" dataDxfId="13" dataCellStyle="Note">
+    <tableColumn id="37" name="End Spatial Cell" dataDxfId="18" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="12" dataCellStyle="Note">
+    <tableColumn id="38" name="Start Spatial Cell" dataDxfId="17" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Delta T" dataDxfId="11" dataCellStyle="Note">
+    <tableColumn id="28" name="Delta T" dataDxfId="16" dataCellStyle="Note">
       <calculatedColumnFormula>Delta_T__seconds</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="Error Ti" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="29" name="Error Ti" dataDxfId="15" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="Error Tp" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="30" name="Error Tp" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="Error Tt" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="31" name="Error Tt" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="Column1" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="32" name="Column1" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="Vi" dataDxfId="6" dataCellStyle="Note">
+    <tableColumn id="33" name="Vi" dataDxfId="11" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="delta Tp" dataDxfId="5" dataCellStyle="Note">
+    <tableColumn id="34" name="delta Tp" dataDxfId="10" dataCellStyle="Note">
       <calculatedColumnFormula>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="Column2" dataDxfId="4" dataCellStyle="Note"/>
-    <tableColumn id="36" name="Column3" dataDxfId="3" dataCellStyle="Note">
+    <tableColumn id="35" name="Column2" dataDxfId="9" dataCellStyle="Note"/>
+    <tableColumn id="36" name="Column3" dataDxfId="8" dataCellStyle="Note">
       <calculatedColumnFormula>'Reach Propertise'!$F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="Column4" dataDxfId="2" dataCellStyle="Note"/>
-    <tableColumn id="41" name="X cells for evaluation and comparison with obsered" dataDxfId="1" dataCellStyle="Note">
+    <tableColumn id="40" name="Column4" dataDxfId="7" dataCellStyle="Note"/>
+    <tableColumn id="41" name="X cells for evaluation and comparison with obsered" dataDxfId="6" dataCellStyle="Note">
       <calculatedColumnFormula>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" name="Observed Concentration [ppm] using formula2" dataDxfId="0" dataCellStyle="Note">
+    <tableColumn id="42" name="Observed Concentration [ppm] using formula2" dataDxfId="5" dataCellStyle="Note">
       <calculatedColumnFormula>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="O2:Q22" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="O2:Q22"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="index" dataDxfId="2"/>
+    <tableColumn id="2" name="Choose From References" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Working?" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4686,7 +4779,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7086,7 +7179,7 @@
   </sheetPr>
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
@@ -7202,7 +7295,7 @@
       <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="95" t="s">
+      <c r="X1" s="89" t="s">
         <v>115</v>
       </c>
       <c r="Y1" s="17" t="s">
@@ -7253,10 +7346,10 @@
       <c r="AN1" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="AO1" s="98" t="s">
+      <c r="AO1" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="AP1" s="98" t="s">
+      <c r="AP1" s="92" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7329,7 +7422,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>0.21</v>
       </c>
-      <c r="X2" s="96">
+      <c r="X2" s="90">
         <v>1.0510314000000001</v>
       </c>
       <c r="Y2" s="76" t="str">
@@ -7394,11 +7487,11 @@
       <c r="AN2" s="75">
         <v>0</v>
       </c>
-      <c r="AO2" s="99">
+      <c r="AO2" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>3</v>
       </c>
-      <c r="AP2" s="99">
+      <c r="AP2" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7472,7 +7565,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>1.175</v>
       </c>
-      <c r="X3" s="96">
+      <c r="X3" s="90">
         <v>0.22527449999999999</v>
       </c>
       <c r="Y3" s="76" t="str">
@@ -7537,11 +7630,11 @@
       <c r="AN3" s="75">
         <v>1</v>
       </c>
-      <c r="AO3" s="99">
+      <c r="AO3" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>19</v>
       </c>
-      <c r="AP3" s="99">
+      <c r="AP3" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7615,7 +7708,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>2.875</v>
       </c>
-      <c r="X4" s="97">
+      <c r="X4" s="91">
         <v>0.11053590000000001</v>
       </c>
       <c r="Y4" s="76" t="str">
@@ -7676,11 +7769,11 @@
         <v>1.1333</v>
       </c>
       <c r="AN4" s="75"/>
-      <c r="AO4" s="99">
+      <c r="AO4" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>47</v>
       </c>
-      <c r="AP4" s="99">
+      <c r="AP4" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7754,7 +7847,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>5.2750000000000004</v>
       </c>
-      <c r="X5" s="97">
+      <c r="X5" s="91">
         <v>5.8002699999999997E-2</v>
       </c>
       <c r="Y5" s="76" t="str">
@@ -7815,11 +7908,11 @@
         <v>2.4666999999999999</v>
       </c>
       <c r="AN5" s="75"/>
-      <c r="AO5" s="99">
+      <c r="AO5" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>87</v>
       </c>
-      <c r="AP5" s="99">
+      <c r="AP5" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -7893,7 +7986,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>7.7750000000000004</v>
       </c>
-      <c r="X6" s="97">
+      <c r="X6" s="91">
         <v>3.4605400000000001E-2</v>
       </c>
       <c r="Y6" s="76" t="str">
@@ -7954,11 +8047,11 @@
         <v>3.7332999999999998</v>
       </c>
       <c r="AN6" s="75"/>
-      <c r="AO6" s="99">
+      <c r="AO6" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>129</v>
       </c>
-      <c r="AP6" s="99">
+      <c r="AP6" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8032,7 +8125,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>10.275</v>
       </c>
-      <c r="X7" s="97">
+      <c r="X7" s="91">
         <v>2.1080000000000002E-2</v>
       </c>
       <c r="Y7" s="76" t="str">
@@ -8093,11 +8186,11 @@
         <v>5.0332999999999997</v>
       </c>
       <c r="AN7" s="75"/>
-      <c r="AO7" s="99">
+      <c r="AO7" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>171</v>
       </c>
-      <c r="AP7" s="99">
+      <c r="AP7" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8171,7 +8264,7 @@
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>13.775</v>
       </c>
-      <c r="X8" s="97">
+      <c r="X8" s="91">
         <v>2.0655E-2</v>
       </c>
       <c r="Y8" s="76" t="str">
@@ -8232,11 +8325,11 @@
         <v>6.5369000000000002</v>
       </c>
       <c r="AN8" s="75"/>
-      <c r="AO8" s="99">
+      <c r="AO8" s="93">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
         <v>229</v>
       </c>
-      <c r="AP8" s="99">
+      <c r="AP8" s="93">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
@@ -8436,235 +8529,365 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+    </row>
+    <row r="2" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="P2" s="89" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="100" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="99" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>66</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="P3" s="90" t="s">
+      <c r="N3" s="95"/>
+      <c r="O3" s="99">
+        <v>1</v>
+      </c>
+      <c r="P3" s="101" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="99" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>62</v>
       </c>
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="P4" s="90" t="s">
+      <c r="N4" s="95"/>
+      <c r="O4" s="99">
+        <v>2</v>
+      </c>
+      <c r="P4" s="101" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="99" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>63</v>
       </c>
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="P5" s="90" t="s">
+      <c r="N5" s="95"/>
+      <c r="O5" s="99">
+        <v>3</v>
+      </c>
+      <c r="P5" s="101" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="99" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>64</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="P6" s="90" t="s">
+      <c r="N6" s="95"/>
+      <c r="O6" s="99">
+        <v>4</v>
+      </c>
+      <c r="P6" s="101" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q6" s="99" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>65</v>
       </c>
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="P7" s="90" t="s">
+      <c r="N7" s="95"/>
+      <c r="O7" s="99">
+        <v>5</v>
+      </c>
+      <c r="P7" s="101" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="99"/>
+    </row>
+    <row r="8" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>67</v>
       </c>
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="P8" s="90" t="s">
+      <c r="N8" s="95"/>
+      <c r="O8" s="99">
+        <v>6</v>
+      </c>
+      <c r="P8" s="101" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="99"/>
+    </row>
+    <row r="9" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>68</v>
       </c>
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="P9" s="90" t="s">
+      <c r="N9" s="95"/>
+      <c r="O9" s="99">
+        <v>7</v>
+      </c>
+      <c r="P9" s="101" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q9" s="99"/>
+    </row>
+    <row r="10" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="P10" s="90" t="s">
+      <c r="N10" s="95"/>
+      <c r="O10" s="99">
+        <v>8</v>
+      </c>
+      <c r="P10" s="101" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="99"/>
+    </row>
+    <row r="11" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="P11" s="90" t="s">
+      <c r="N11" s="95"/>
+      <c r="O11" s="99">
+        <v>9</v>
+      </c>
+      <c r="P11" s="101" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="99"/>
+    </row>
+    <row r="12" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="P12" s="91" t="s">
+      <c r="N12" s="95"/>
+      <c r="O12" s="99">
+        <v>10</v>
+      </c>
+      <c r="P12" s="102" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="99"/>
+    </row>
+    <row r="13" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="P13" s="90" t="s">
+      <c r="N13" s="95"/>
+      <c r="O13" s="99">
+        <v>11</v>
+      </c>
+      <c r="P13" s="101" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="99"/>
+    </row>
+    <row r="14" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="P14" s="90" t="s">
+      <c r="N14" s="95"/>
+      <c r="O14" s="99">
+        <v>12</v>
+      </c>
+      <c r="P14" s="101" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="99"/>
+    </row>
+    <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="P15" s="90" t="s">
+      <c r="N15" s="95"/>
+      <c r="O15" s="99">
+        <v>13</v>
+      </c>
+      <c r="P15" s="101" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q15" s="99"/>
+    </row>
+    <row r="16" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="P16" s="90" t="s">
+      <c r="N16" s="95"/>
+      <c r="O16" s="99">
+        <v>14</v>
+      </c>
+      <c r="P16" s="101" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="99"/>
+    </row>
+    <row r="17" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="P17" s="90" t="s">
+      <c r="N17" s="95"/>
+      <c r="O17" s="99">
+        <v>15</v>
+      </c>
+      <c r="P17" s="101" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="99"/>
+    </row>
+    <row r="18" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="P18" s="90" t="s">
+      <c r="N18" s="95"/>
+      <c r="O18" s="99">
+        <v>16</v>
+      </c>
+      <c r="P18" s="101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q18" s="99"/>
+    </row>
+    <row r="19" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="P19" s="90" t="s">
+      <c r="N19" s="95"/>
+      <c r="O19" s="99">
+        <v>17</v>
+      </c>
+      <c r="P19" s="101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="99"/>
+    </row>
+    <row r="20" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="P20" s="90" t="s">
+      <c r="N20" s="95"/>
+      <c r="O20" s="99">
+        <v>18</v>
+      </c>
+      <c r="P20" s="101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="99"/>
+    </row>
+    <row r="21" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H21">
         <v>900</v>
       </c>
-      <c r="P21" s="90" t="s">
+      <c r="N21" s="95"/>
+      <c r="O21" s="99">
+        <v>19</v>
+      </c>
+      <c r="P21" s="101" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="99"/>
+    </row>
+    <row r="22" spans="8:17" ht="21" x14ac:dyDescent="0.35">
       <c r="H22">
         <v>1000</v>
       </c>
-      <c r="P22" s="92" t="s">
+      <c r="N22" s="95"/>
+      <c r="O22" s="99">
+        <v>20</v>
+      </c>
+      <c r="P22" s="102" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="23" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="99"/>
+    </row>
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="P23" s="92"/>
-    </row>
-    <row r="24" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="95"/>
+    </row>
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1500</v>
       </c>
-      <c r="P24" s="93"/>
-    </row>
-    <row r="25" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="P25" s="94"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="96"/>
+      <c r="Q24" s="95"/>
+    </row>
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="98"/>
+      <c r="Q25" s="95"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8689,6 +8912,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -8696,68 +8922,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="J1" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="K1" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="L1" s="94" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="M1" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="N1" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="O1" s="94" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="P1" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="Q1" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="R1" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="S1" s="94" t="s">
         <v>102</v>
       </c>
     </row>
@@ -9779,15 +10005,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="44"/>
-      <c r="G28" s="100" t="s">
+      <c r="G28" s="103" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="101"/>
-      <c r="I28" s="101"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="102"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="45" t="s">

</xml_diff>